<commit_message>
modified:   BUILD/Linux/ewlog/usr/share/ewlog/serviceLOG.db 	modified:   BUILD/x64/serviceLOG.db 	modified:   BUILD/x86/serviceLOG.db 	modified:   RDA.xlsx 	modified:   URDA.xlsx 	modified:   WDRB.xlsx 	modified:   serviceLOG.db
</commit_message>
<xml_diff>
--- a/WDRB.xlsx
+++ b/WDRB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EWLog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vkarpenko\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="287">
   <si>
     <t>CT</t>
   </si>
@@ -885,15 +885,12 @@
   </si>
   <si>
     <t>ВЕТКОВСКИЙ</t>
-  </si>
-  <si>
-    <t>Numb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -926,7 +923,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -934,53 +931,20 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1263,1738 +1227,1595 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D144"/>
+  <dimension ref="A1:C144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="33.140625" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="33.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C1" t="s">
-        <v>287</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C1" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="4" t="s">
+      <c r="C23" s="3" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="4" t="s">
+      <c r="C25" s="3" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="4" t="s">
+      <c r="C26" s="3" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="4" t="s">
+      <c r="C27" s="3" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="4" t="s">
+      <c r="C28" s="3" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="4" t="s">
+      <c r="C29" s="3" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="4" t="s">
+      <c r="C30" s="3" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="4" t="s">
+      <c r="C31" s="3" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="4" t="s">
+      <c r="C32" s="3" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="4" t="s">
+      <c r="C33" s="3" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="4" t="s">
+      <c r="C34" s="3" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="4" t="s">
+      <c r="C35" s="3" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="4" t="s">
+      <c r="C36" s="3" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="4" t="s">
+      <c r="C37" s="3" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C38" s="2"/>
-      <c r="D38" s="4" t="s">
+      <c r="C38" s="3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C39" s="2"/>
-      <c r="D39" s="4" t="s">
+      <c r="C39" s="3" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="2"/>
-      <c r="D40" s="4" t="s">
+      <c r="C40" s="3" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C41" s="2"/>
-      <c r="D41" s="4" t="s">
+      <c r="C41" s="3" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C42" s="2"/>
-      <c r="D42" s="4" t="s">
+      <c r="C42" s="3" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C43" s="2"/>
-      <c r="D43" s="4" t="s">
+      <c r="C43" s="3" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C44" s="2"/>
-      <c r="D44" s="4" t="s">
+      <c r="C44" s="3" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C45" s="2"/>
-      <c r="D45" s="4" t="s">
+      <c r="C45" s="3" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C46" s="2"/>
-      <c r="D46" s="4" t="s">
+      <c r="C46" s="3" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C47" s="2"/>
-      <c r="D47" s="4" t="s">
+      <c r="C47" s="3" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="2"/>
-      <c r="D48" s="4" t="s">
+      <c r="C48" s="3" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C49" s="2"/>
-      <c r="D49" s="4" t="s">
+      <c r="C49" s="3" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C50" s="2"/>
-      <c r="D50" s="4" t="s">
+      <c r="C50" s="3" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C51" s="2"/>
-      <c r="D51" s="4" t="s">
+      <c r="C51" s="3" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C52" s="2"/>
-      <c r="D52" s="4" t="s">
+      <c r="C52" s="3" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C53" s="2"/>
-      <c r="D53" s="4" t="s">
+      <c r="C53" s="3" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C54" s="2"/>
-      <c r="D54" s="4" t="s">
+      <c r="C54" s="3" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C55" s="2"/>
-      <c r="D55" s="4" t="s">
+      <c r="C55" s="3" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C56" s="2"/>
-      <c r="D56" s="4" t="s">
+      <c r="C56" s="3" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
         <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C57" s="2"/>
-      <c r="D57" s="4" t="s">
+      <c r="C57" s="3" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
         <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C58" s="2"/>
-      <c r="D58" s="4" t="s">
+      <c r="C58" s="3" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
         <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C59" s="2"/>
-      <c r="D59" s="4" t="s">
+      <c r="C59" s="3" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
         <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C60" s="2"/>
-      <c r="D60" s="4" t="s">
+      <c r="C60" s="3" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
         <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C61" s="2"/>
-      <c r="D61" s="4" t="s">
+      <c r="C61" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
         <v>61</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C62" s="2"/>
-      <c r="D62" s="4" t="s">
+      <c r="C62" s="3" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
         <v>62</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C63" s="2"/>
-      <c r="D63" s="4" t="s">
+      <c r="C63" s="3" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
         <v>63</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C64" s="2"/>
-      <c r="D64" s="4" t="s">
+      <c r="C64" s="3" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
         <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C65" s="2"/>
-      <c r="D65" s="4" t="s">
+      <c r="C65" s="3" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
         <v>65</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C66" s="2"/>
-      <c r="D66" s="4" t="s">
+      <c r="C66" s="3" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
         <v>66</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C67" s="2"/>
-      <c r="D67" s="4" t="s">
+      <c r="C67" s="3" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
         <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C68" s="2"/>
-      <c r="D68" s="4" t="s">
+      <c r="C68" s="3" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
         <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C69" s="2"/>
-      <c r="D69" s="4" t="s">
+      <c r="C69" s="3" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
         <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C70" s="2"/>
-      <c r="D70" s="4" t="s">
+      <c r="C70" s="3" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
         <v>70</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C71" s="2"/>
-      <c r="D71" s="4" t="s">
+      <c r="C71" s="3" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
         <v>71</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C72" s="2"/>
-      <c r="D72" s="4" t="s">
+      <c r="C72" s="3" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
         <v>72</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C73" s="2"/>
-      <c r="D73" s="4" t="s">
+      <c r="C73" s="3" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
         <v>73</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C74" s="2"/>
-      <c r="D74" s="4" t="s">
+      <c r="C74" s="3" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
         <v>74</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C75" s="2"/>
-      <c r="D75" s="4" t="s">
+      <c r="C75" s="3" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
         <v>75</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C76" s="2"/>
-      <c r="D76" s="4" t="s">
+      <c r="C76" s="3" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
         <v>76</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C77" s="2"/>
-      <c r="D77" s="4" t="s">
+      <c r="C77" s="3" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
         <v>77</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C78" s="2"/>
-      <c r="D78" s="4" t="s">
+      <c r="C78" s="3" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
         <v>78</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C79" s="2"/>
-      <c r="D79" s="4" t="s">
+      <c r="C79" s="3" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
         <v>79</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C80" s="2"/>
-      <c r="D80" s="4" t="s">
+      <c r="C80" s="3" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
         <v>80</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C81" s="2"/>
-      <c r="D81" s="4" t="s">
+      <c r="C81" s="3" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
         <v>81</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C82" s="2"/>
-      <c r="D82" s="4" t="s">
+      <c r="C82" s="3" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
         <v>82</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C83" s="2"/>
-      <c r="D83" s="4" t="s">
+      <c r="C83" s="3" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
         <v>83</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C84" s="2"/>
-      <c r="D84" s="4" t="s">
+      <c r="C84" s="3" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
         <v>84</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C85" s="2"/>
-      <c r="D85" s="4" t="s">
+      <c r="C85" s="3" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
         <v>85</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C86" s="2"/>
-      <c r="D86" s="4" t="s">
+      <c r="C86" s="3" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
         <v>86</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C87" s="2"/>
-      <c r="D87" s="4" t="s">
+      <c r="C87" s="3" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
         <v>87</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C88" s="2"/>
-      <c r="D88" s="4" t="s">
+      <c r="C88" s="3" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
         <v>88</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C89" s="2"/>
-      <c r="D89" s="4" t="s">
+      <c r="C89" s="3" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
         <v>89</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C90" s="2"/>
-      <c r="D90" s="4" t="s">
+      <c r="C90" s="3" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
         <v>90</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C91" s="2"/>
-      <c r="D91" s="4" t="s">
+      <c r="C91" s="3" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A92">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
         <v>91</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C92" s="2"/>
-      <c r="D92" s="4" t="s">
+      <c r="C92" s="3" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
         <v>92</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C93" s="2"/>
-      <c r="D93" s="4" t="s">
+      <c r="C93" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
         <v>93</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C94" s="2"/>
-      <c r="D94" s="4" t="s">
+      <c r="C94" s="3" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
         <v>94</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C95" s="2"/>
-      <c r="D95" s="4" t="s">
+      <c r="C95" s="3" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A96">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
         <v>95</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C96" s="2"/>
-      <c r="D96" s="4" t="s">
+      <c r="C96" s="3" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
         <v>96</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C97" s="2"/>
-      <c r="D97" s="4" t="s">
+      <c r="C97" s="3" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
         <v>97</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C98" s="2"/>
-      <c r="D98" s="4" t="s">
+      <c r="C98" s="3" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
         <v>98</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C99" s="2"/>
-      <c r="D99" s="4" t="s">
+      <c r="C99" s="3" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
         <v>99</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C100" s="2"/>
-      <c r="D100" s="4" t="s">
+      <c r="C100" s="3" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
         <v>100</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C101" s="2"/>
-      <c r="D101" s="4" t="s">
+      <c r="C101" s="3" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A102">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
         <v>101</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C102" s="2"/>
-      <c r="D102" s="4" t="s">
+      <c r="C102" s="3" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
         <v>102</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C103" s="2"/>
-      <c r="D103" s="4" t="s">
+      <c r="C103" s="3" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
         <v>103</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C104" s="2"/>
-      <c r="D104" s="4" t="s">
+      <c r="C104" s="3" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
         <v>104</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C105" s="2"/>
-      <c r="D105" s="4" t="s">
+      <c r="C105" s="3" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
         <v>105</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C106" s="2"/>
-      <c r="D106" s="4" t="s">
+      <c r="C106" s="3" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
         <v>106</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C107" s="2"/>
-      <c r="D107" s="4" t="s">
+      <c r="C107" s="3" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="1">
         <v>107</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C108" s="2"/>
-      <c r="D108" s="4" t="s">
+      <c r="C108" s="3" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
         <v>108</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C109" s="2"/>
-      <c r="D109" s="4" t="s">
+      <c r="C109" s="3" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
         <v>109</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C110" s="2"/>
-      <c r="D110" s="4" t="s">
+      <c r="C110" s="3" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
         <v>110</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C111" s="2"/>
-      <c r="D111" s="4" t="s">
+      <c r="C111" s="3" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A112">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
         <v>111</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C112" s="2"/>
-      <c r="D112" s="4" t="s">
+      <c r="C112" s="3" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="1">
         <v>112</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C113" s="2"/>
-      <c r="D113" s="4" t="s">
+      <c r="C113" s="3" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A114">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
         <v>113</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C114" s="2"/>
-      <c r="D114" s="4" t="s">
+      <c r="C114" s="3" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A115">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
         <v>114</v>
       </c>
       <c r="B115" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C115" s="2"/>
-      <c r="D115" s="4" t="s">
+      <c r="C115" s="3" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A116">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="1">
         <v>115</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C116" s="2"/>
-      <c r="D116" s="4" t="s">
+      <c r="C116" s="3" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="1">
         <v>116</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C117" s="2"/>
-      <c r="D117" s="4" t="s">
+      <c r="C117" s="3" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A118">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="1">
         <v>117</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C118" s="2"/>
-      <c r="D118" s="4" t="s">
+      <c r="C118" s="3" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A119">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="1">
         <v>118</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C119" s="2"/>
-      <c r="D119" s="4" t="s">
+      <c r="C119" s="3" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A120">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="1">
         <v>119</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C120" s="2"/>
-      <c r="D120" s="4" t="s">
+      <c r="C120" s="3" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="1">
         <v>120</v>
       </c>
       <c r="B121" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C121" s="2"/>
-      <c r="D121" s="4" t="s">
+      <c r="C121" s="3" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A122">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="1">
         <v>121</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C122" s="2"/>
-      <c r="D122" s="4" t="s">
+      <c r="C122" s="3" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="1">
         <v>122</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C123" s="2"/>
-      <c r="D123" s="4" t="s">
+      <c r="C123" s="3" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A124">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="1">
         <v>123</v>
       </c>
       <c r="B124" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C124" s="2"/>
-      <c r="D124" s="4" t="s">
+      <c r="C124" s="3" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A125">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="1">
         <v>124</v>
       </c>
       <c r="B125" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C125" s="2"/>
-      <c r="D125" s="4" t="s">
+      <c r="C125" s="3" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A126">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="1">
         <v>125</v>
       </c>
       <c r="B126" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C126" s="2"/>
-      <c r="D126" s="4" t="s">
+      <c r="C126" s="3" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A127">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="1">
         <v>126</v>
       </c>
       <c r="B127" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C127" s="2"/>
-      <c r="D127" s="4" t="s">
+      <c r="C127" s="3" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A128">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="1">
         <v>127</v>
       </c>
       <c r="B128" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C128" s="2"/>
-      <c r="D128" s="4" t="s">
+      <c r="C128" s="3" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="1">
         <v>128</v>
       </c>
       <c r="B129" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C129" s="2"/>
-      <c r="D129" s="4" t="s">
+      <c r="C129" s="3" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A130">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="1">
         <v>129</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C130" s="2"/>
-      <c r="D130" s="4" t="s">
+      <c r="C130" s="3" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A131">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="1">
         <v>130</v>
       </c>
       <c r="B131" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C131" s="2"/>
-      <c r="D131" s="4" t="s">
+      <c r="C131" s="3" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A132">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="1">
         <v>131</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C132" s="2"/>
-      <c r="D132" s="4" t="s">
+      <c r="C132" s="3" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="1">
         <v>132</v>
       </c>
       <c r="B133" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C133" s="2"/>
-      <c r="D133" s="4" t="s">
+      <c r="C133" s="3" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A134">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="1">
         <v>133</v>
       </c>
       <c r="B134" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C134" s="2"/>
-      <c r="D134" s="4" t="s">
+      <c r="C134" s="3" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A135">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="1">
         <v>134</v>
       </c>
       <c r="B135" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C135" s="2"/>
-      <c r="D135" s="4" t="s">
+      <c r="C135" s="3" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A136">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="1">
         <v>135</v>
       </c>
       <c r="B136" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C136" s="2"/>
-      <c r="D136" s="4" t="s">
+      <c r="C136" s="3" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A137">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="1">
         <v>136</v>
       </c>
       <c r="B137" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C137" s="2"/>
-      <c r="D137" s="4" t="s">
+      <c r="C137" s="3" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A138">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="1">
         <v>137</v>
       </c>
       <c r="B138" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C138" s="2"/>
-      <c r="D138" s="4" t="s">
+      <c r="C138" s="3" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A139">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="1">
         <v>138</v>
       </c>
       <c r="B139" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C139" s="2"/>
-      <c r="D139" s="4" t="s">
+      <c r="C139" s="3" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A140">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="1">
         <v>139</v>
       </c>
       <c r="B140" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C140" s="2"/>
-      <c r="D140" s="4" t="s">
+      <c r="C140" s="3" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A141">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="1">
         <v>140</v>
       </c>
       <c r="B141" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C141" s="2"/>
-      <c r="D141" s="4" t="s">
+      <c r="C141" s="3" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A142">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="1">
         <v>141</v>
       </c>
       <c r="B142" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C142" s="2"/>
-      <c r="D142" s="4" t="s">
+      <c r="C142" s="3" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A143">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" s="1">
         <v>142</v>
       </c>
       <c r="B143" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C143" s="2"/>
-      <c r="D143" s="4" t="s">
+      <c r="C143" s="3" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D144" s="5"/>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C144" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>